<commit_message>
correct some error in Schedule
</commit_message>
<xml_diff>
--- a/PBT-Booking-traveling-/Docs/Sprints-Schedule.xlsx
+++ b/PBT-Booking-traveling-/Docs/Sprints-Schedule.xlsx
@@ -1386,9 +1386,6 @@
     <t xml:space="preserve">Ahmed Adel </t>
   </si>
   <si>
-    <t>…………..</t>
-  </si>
-  <si>
     <t>Ibrahim rashed</t>
   </si>
   <si>
@@ -1462,6 +1459,9 @@
   </si>
   <si>
     <t>Sprint 3 OffersSection</t>
+  </si>
+  <si>
+    <t>Ebrahim Rashed &amp; Eid</t>
   </si>
 </sst>
 </file>
@@ -2643,6 +2643,9 @@
     <xf numFmtId="0" fontId="62" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2660,9 +2663,6 @@
     </xf>
     <xf numFmtId="166" fontId="41" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2714,111 +2714,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -3018,7 +2914,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3070,7 +2966,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>24</xdr:col>
-          <xdr:colOff>104776</xdr:colOff>
+          <xdr:colOff>104775</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -3082,7 +2978,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3132,7 +3028,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3216,7 +3112,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3271,7 +3167,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3326,7 +3222,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3654,8 +3550,8 @@
   <dimension ref="A1:BK45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3678,29 +3574,29 @@
       <c r="B1" s="41"/>
       <c r="C1" s="41"/>
       <c r="F1" s="91"/>
-      <c r="H1" s="134" t="s">
+      <c r="H1" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="134"/>
-      <c r="P1" s="134"/>
-      <c r="Q1" s="134"/>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
-      <c r="T1" s="134"/>
-      <c r="U1" s="134"/>
-      <c r="V1" s="134"/>
-      <c r="W1" s="134"/>
-      <c r="X1" s="134"/>
-      <c r="Y1" s="134"/>
-      <c r="Z1" s="134"/>
-      <c r="AA1" s="134"/>
-      <c r="AB1" s="134"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="128"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
+      <c r="Y1" s="128"/>
+      <c r="Z1" s="128"/>
+      <c r="AA1" s="128"/>
+      <c r="AB1" s="128"/>
     </row>
     <row r="2" spans="1:63" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
@@ -3750,86 +3646,86 @@
       </c>
       <c r="F4" s="77"/>
       <c r="G4" s="44"/>
-      <c r="H4" s="128" t="str">
+      <c r="H4" s="129" t="str">
         <f>"Week "&amp;(H6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="130"/>
-      <c r="O4" s="128" t="str">
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="129" t="str">
         <f>"Week "&amp;(O6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="P4" s="129"/>
-      <c r="Q4" s="129"/>
-      <c r="R4" s="129"/>
-      <c r="S4" s="129"/>
-      <c r="T4" s="129"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="128" t="str">
+      <c r="P4" s="130"/>
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="129" t="str">
         <f>"Week "&amp;(V6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="W4" s="129"/>
-      <c r="X4" s="129"/>
-      <c r="Y4" s="129"/>
-      <c r="Z4" s="129"/>
-      <c r="AA4" s="129"/>
-      <c r="AB4" s="130"/>
-      <c r="AC4" s="128" t="str">
+      <c r="W4" s="130"/>
+      <c r="X4" s="130"/>
+      <c r="Y4" s="130"/>
+      <c r="Z4" s="130"/>
+      <c r="AA4" s="130"/>
+      <c r="AB4" s="131"/>
+      <c r="AC4" s="129" t="str">
         <f>"Week "&amp;(AC6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AD4" s="129"/>
-      <c r="AE4" s="129"/>
-      <c r="AF4" s="129"/>
-      <c r="AG4" s="129"/>
-      <c r="AH4" s="129"/>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="128" t="str">
+      <c r="AD4" s="130"/>
+      <c r="AE4" s="130"/>
+      <c r="AF4" s="130"/>
+      <c r="AG4" s="130"/>
+      <c r="AH4" s="130"/>
+      <c r="AI4" s="131"/>
+      <c r="AJ4" s="129" t="str">
         <f>"Week "&amp;(AJ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AK4" s="129"/>
-      <c r="AL4" s="129"/>
-      <c r="AM4" s="129"/>
-      <c r="AN4" s="129"/>
-      <c r="AO4" s="129"/>
-      <c r="AP4" s="130"/>
-      <c r="AQ4" s="128" t="str">
+      <c r="AK4" s="130"/>
+      <c r="AL4" s="130"/>
+      <c r="AM4" s="130"/>
+      <c r="AN4" s="130"/>
+      <c r="AO4" s="130"/>
+      <c r="AP4" s="131"/>
+      <c r="AQ4" s="129" t="str">
         <f>"Week "&amp;(AQ6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AR4" s="129"/>
-      <c r="AS4" s="129"/>
-      <c r="AT4" s="129"/>
-      <c r="AU4" s="129"/>
-      <c r="AV4" s="129"/>
-      <c r="AW4" s="130"/>
-      <c r="AX4" s="128" t="str">
+      <c r="AR4" s="130"/>
+      <c r="AS4" s="130"/>
+      <c r="AT4" s="130"/>
+      <c r="AU4" s="130"/>
+      <c r="AV4" s="130"/>
+      <c r="AW4" s="131"/>
+      <c r="AX4" s="129" t="str">
         <f>"Week "&amp;(AX6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AY4" s="129"/>
-      <c r="AZ4" s="129"/>
-      <c r="BA4" s="129"/>
-      <c r="BB4" s="129"/>
-      <c r="BC4" s="129"/>
-      <c r="BD4" s="130"/>
-      <c r="BE4" s="128" t="str">
+      <c r="AY4" s="130"/>
+      <c r="AZ4" s="130"/>
+      <c r="BA4" s="130"/>
+      <c r="BB4" s="130"/>
+      <c r="BC4" s="130"/>
+      <c r="BD4" s="131"/>
+      <c r="BE4" s="129" t="str">
         <f>"Week "&amp;(BE6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BF4" s="129"/>
-      <c r="BG4" s="129"/>
-      <c r="BH4" s="129"/>
-      <c r="BI4" s="129"/>
-      <c r="BJ4" s="129"/>
-      <c r="BK4" s="130"/>
+      <c r="BF4" s="130"/>
+      <c r="BG4" s="130"/>
+      <c r="BH4" s="130"/>
+      <c r="BI4" s="130"/>
+      <c r="BJ4" s="130"/>
+      <c r="BK4" s="131"/>
     </row>
     <row r="5" spans="1:63" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76"/>
@@ -3841,86 +3737,86 @@
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
       <c r="G5" s="44"/>
-      <c r="H5" s="131">
+      <c r="H5" s="132">
         <f>H6</f>
         <v>43157</v>
       </c>
-      <c r="I5" s="132"/>
-      <c r="J5" s="132"/>
-      <c r="K5" s="132"/>
-      <c r="L5" s="132"/>
-      <c r="M5" s="132"/>
-      <c r="N5" s="133"/>
-      <c r="O5" s="131">
+      <c r="I5" s="133"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="132">
         <f>O6</f>
         <v>43164</v>
       </c>
-      <c r="P5" s="132"/>
-      <c r="Q5" s="132"/>
-      <c r="R5" s="132"/>
-      <c r="S5" s="132"/>
-      <c r="T5" s="132"/>
-      <c r="U5" s="133"/>
-      <c r="V5" s="131">
+      <c r="P5" s="133"/>
+      <c r="Q5" s="133"/>
+      <c r="R5" s="133"/>
+      <c r="S5" s="133"/>
+      <c r="T5" s="133"/>
+      <c r="U5" s="134"/>
+      <c r="V5" s="132">
         <f>V6</f>
         <v>43171</v>
       </c>
-      <c r="W5" s="132"/>
-      <c r="X5" s="132"/>
-      <c r="Y5" s="132"/>
-      <c r="Z5" s="132"/>
-      <c r="AA5" s="132"/>
-      <c r="AB5" s="133"/>
-      <c r="AC5" s="131">
+      <c r="W5" s="133"/>
+      <c r="X5" s="133"/>
+      <c r="Y5" s="133"/>
+      <c r="Z5" s="133"/>
+      <c r="AA5" s="133"/>
+      <c r="AB5" s="134"/>
+      <c r="AC5" s="132">
         <f>AC6</f>
         <v>43178</v>
       </c>
-      <c r="AD5" s="132"/>
-      <c r="AE5" s="132"/>
-      <c r="AF5" s="132"/>
-      <c r="AG5" s="132"/>
-      <c r="AH5" s="132"/>
-      <c r="AI5" s="133"/>
-      <c r="AJ5" s="131">
+      <c r="AD5" s="133"/>
+      <c r="AE5" s="133"/>
+      <c r="AF5" s="133"/>
+      <c r="AG5" s="133"/>
+      <c r="AH5" s="133"/>
+      <c r="AI5" s="134"/>
+      <c r="AJ5" s="132">
         <f>AJ6</f>
         <v>43185</v>
       </c>
-      <c r="AK5" s="132"/>
-      <c r="AL5" s="132"/>
-      <c r="AM5" s="132"/>
-      <c r="AN5" s="132"/>
-      <c r="AO5" s="132"/>
-      <c r="AP5" s="133"/>
-      <c r="AQ5" s="131">
+      <c r="AK5" s="133"/>
+      <c r="AL5" s="133"/>
+      <c r="AM5" s="133"/>
+      <c r="AN5" s="133"/>
+      <c r="AO5" s="133"/>
+      <c r="AP5" s="134"/>
+      <c r="AQ5" s="132">
         <f>AQ6</f>
         <v>43192</v>
       </c>
-      <c r="AR5" s="132"/>
-      <c r="AS5" s="132"/>
-      <c r="AT5" s="132"/>
-      <c r="AU5" s="132"/>
-      <c r="AV5" s="132"/>
-      <c r="AW5" s="133"/>
-      <c r="AX5" s="131">
+      <c r="AR5" s="133"/>
+      <c r="AS5" s="133"/>
+      <c r="AT5" s="133"/>
+      <c r="AU5" s="133"/>
+      <c r="AV5" s="133"/>
+      <c r="AW5" s="134"/>
+      <c r="AX5" s="132">
         <f>AX6</f>
         <v>43199</v>
       </c>
-      <c r="AY5" s="132"/>
-      <c r="AZ5" s="132"/>
-      <c r="BA5" s="132"/>
-      <c r="BB5" s="132"/>
-      <c r="BC5" s="132"/>
-      <c r="BD5" s="133"/>
-      <c r="BE5" s="131">
+      <c r="AY5" s="133"/>
+      <c r="AZ5" s="133"/>
+      <c r="BA5" s="133"/>
+      <c r="BB5" s="133"/>
+      <c r="BC5" s="133"/>
+      <c r="BD5" s="134"/>
+      <c r="BE5" s="132">
         <f>BE6</f>
         <v>43206</v>
       </c>
-      <c r="BF5" s="132"/>
-      <c r="BG5" s="132"/>
-      <c r="BH5" s="132"/>
-      <c r="BI5" s="132"/>
-      <c r="BJ5" s="132"/>
-      <c r="BK5" s="133"/>
+      <c r="BF5" s="133"/>
+      <c r="BG5" s="133"/>
+      <c r="BH5" s="133"/>
+      <c r="BI5" s="133"/>
+      <c r="BJ5" s="133"/>
+      <c r="BK5" s="134"/>
     </row>
     <row r="6" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A6" s="43"/>
@@ -4406,7 +4302,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="62"/>
       <c r="D8" s="63"/>
@@ -4476,7 +4372,7 @@
         <v>1.1</v>
       </c>
       <c r="B9" s="88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>129</v>
@@ -4945,7 +4841,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="54">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F15" s="55">
         <v>2</v>
@@ -5254,7 +5150,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="54">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F19" s="55">
         <v>5</v>
@@ -5401,16 +5297,16 @@
         <v>1.6</v>
       </c>
       <c r="B21" s="88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D21" s="53">
         <v>4</v>
       </c>
       <c r="E21" s="54">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F21" s="55">
         <v>3</v>
@@ -5479,7 +5375,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="50"/>
@@ -5548,10 +5444,10 @@
         <v>2.1</v>
       </c>
       <c r="B23" s="88" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" s="53">
         <v>4</v>
@@ -5626,7 +5522,7 @@
         <v>2.2</v>
       </c>
       <c r="B24" s="88" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>148</v>
@@ -5702,7 +5598,7 @@
         <v>2.3</v>
       </c>
       <c r="B25" s="88" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="52" t="s">
         <v>134</v>
@@ -5778,7 +5674,7 @@
         <v>2.4</v>
       </c>
       <c r="B26" s="88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>134</v>
@@ -5853,10 +5749,10 @@
         <v>2.5</v>
       </c>
       <c r="B27" s="88" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" s="52" t="s">
         <v>157</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>158</v>
       </c>
       <c r="D27" s="53">
         <v>8</v>
@@ -5931,10 +5827,10 @@
         <v>2.6</v>
       </c>
       <c r="B28" s="88" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D28" s="53">
         <v>3</v>
@@ -6009,7 +5905,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D29" s="49"/>
       <c r="E29" s="50"/>
@@ -6078,10 +5974,10 @@
         <v>3.1</v>
       </c>
       <c r="B30" s="88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" s="52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" s="53">
         <v>8</v>
@@ -6156,10 +6052,10 @@
         <v>3.2</v>
       </c>
       <c r="B31" s="88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C31" s="52" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D31" s="53">
         <v>6</v>
@@ -6234,10 +6130,10 @@
         <v>3.3</v>
       </c>
       <c r="B32" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="52" t="s">
         <v>169</v>
-      </c>
-      <c r="C32" s="52" t="s">
-        <v>170</v>
       </c>
       <c r="D32" s="53">
         <v>3</v>
@@ -6312,7 +6208,7 @@
         <v>3.4</v>
       </c>
       <c r="B33" s="88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>134</v>
@@ -6389,10 +6285,10 @@
         <v>3.5</v>
       </c>
       <c r="B34" s="88" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="52" t="s">
         <v>159</v>
-      </c>
-      <c r="C34" s="52" t="s">
-        <v>160</v>
       </c>
       <c r="D34" s="53">
         <v>3</v>
@@ -6467,10 +6363,10 @@
         <v>3.6</v>
       </c>
       <c r="B35" s="88" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="52" t="s">
         <v>175</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>176</v>
       </c>
       <c r="D35" s="53">
         <v>1</v>
@@ -6545,10 +6441,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D36" s="49"/>
       <c r="E36" s="50"/>
@@ -6981,10 +6877,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="48" t="s">
         <v>172</v>
-      </c>
-      <c r="C42" s="48" t="s">
-        <v>173</v>
       </c>
       <c r="D42" s="49"/>
       <c r="E42" s="50"/>
@@ -7248,13 +7144,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="17">
-    <mergeCell ref="H1:AB1"/>
-    <mergeCell ref="O4:U4"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="V5:AB5"/>
     <mergeCell ref="AC4:AI4"/>
     <mergeCell ref="AC5:AI5"/>
     <mergeCell ref="BE4:BK4"/>
@@ -7265,6 +7154,13 @@
     <mergeCell ref="AJ4:AP4"/>
     <mergeCell ref="AX4:BD4"/>
     <mergeCell ref="AX5:BD5"/>
+    <mergeCell ref="H1:AB1"/>
+    <mergeCell ref="O4:U4"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="V5:AB5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E8:E41 E43:E44">
@@ -7282,20 +7178,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:BK7">
-    <cfRule type="expression" dxfId="21" priority="53">
+    <cfRule type="expression" dxfId="9" priority="53">
       <formula>H$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:BK41 H43:BK44">
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>H$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:BK41 H43:BK44">
-    <cfRule type="expression" dxfId="19" priority="60">
+    <cfRule type="expression" dxfId="7" priority="60">
       <formula>AND(#REF!&lt;=H$6,ROUNDDOWN((#REF!-#REF!+1)*$E8,0)+#REF!-1&gt;=H$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="61">
+    <cfRule type="expression" dxfId="6" priority="61">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=H$6,#REF!&gt;=H$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7314,15 +7210,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42:BK42">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>H$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42:BK42">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>AND(#REF!&lt;=H$6,ROUNDDOWN((#REF!-#REF!+1)*$E42,0)+#REF!-1&gt;=H$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=H$6,#REF!&gt;=H$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7341,15 +7237,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:BK45">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>H$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45:BK45">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND(#REF!&lt;=H$6,ROUNDDOWN((#REF!-#REF!+1)*$E45,0)+#REF!-1&gt;=H$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=H$6,#REF!&gt;=H$6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>